<commit_message>
updated email message, prevented 0.00 value invoices form sending
</commit_message>
<xml_diff>
--- a/database/emailfile.xlsx
+++ b/database/emailfile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalee\projects\Auto-Invoicer\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1755E3E-90C3-4E2F-871A-8624B65C4A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256A5FF8-78E3-420A-A3BE-8EC8EDE0805E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30945" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{39A6E6E2-FF2D-434E-96EE-69BD8AE98EE3}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11175" xr2:uid="{39A6E6E2-FF2D-434E-96EE-69BD8AE98EE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="105">
   <si>
     <t>Email</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Customer #</t>
   </si>
   <si>
-    <t>kobiatlaslee@gmail.com</t>
-  </si>
-  <si>
     <t>ACTGREROS</t>
   </si>
   <si>
@@ -57,6 +54,303 @@
   </si>
   <si>
     <t>BOWIEL</t>
+  </si>
+  <si>
+    <t>rob@portamini.com</t>
+  </si>
+  <si>
+    <t>330mgr@activegreenross.com</t>
+  </si>
+  <si>
+    <t>payables@bardonsupplies.com</t>
+  </si>
+  <si>
+    <t>belinda@brystsoccer.com</t>
+  </si>
+  <si>
+    <t>BRYSTFOOT</t>
+  </si>
+  <si>
+    <t>GLOPET</t>
+  </si>
+  <si>
+    <t>globalpetfoodswhitby@gmail.com</t>
+  </si>
+  <si>
+    <t>GALLOSMOT</t>
+  </si>
+  <si>
+    <t>peter@gallos.ca</t>
+  </si>
+  <si>
+    <t>ap@canadianstage.com</t>
+  </si>
+  <si>
+    <t>CANSTAGE</t>
+  </si>
+  <si>
+    <t>accountspayable@cantechelevators.com</t>
+  </si>
+  <si>
+    <t>CANTELE</t>
+  </si>
+  <si>
+    <t>CMPELE</t>
+  </si>
+  <si>
+    <t>cmpelectric@rogers.com</t>
+  </si>
+  <si>
+    <t>mcoles803@gmail.com</t>
+  </si>
+  <si>
+    <t>COLEM</t>
+  </si>
+  <si>
+    <t>CONTEKGRO</t>
+  </si>
+  <si>
+    <t>contekbuildinggroup@bellnet.ca, gheath.contek@gmail.com</t>
+  </si>
+  <si>
+    <t>DURDSB</t>
+  </si>
+  <si>
+    <t>CITBRAMPTN</t>
+  </si>
+  <si>
+    <t>FAIRVIEW</t>
+  </si>
+  <si>
+    <t>Carly-Lynn.Robertson@durham.ca</t>
+  </si>
+  <si>
+    <t>russ@thebrockhouse.ca</t>
+  </si>
+  <si>
+    <t>HOTROC</t>
+  </si>
+  <si>
+    <t>HUMCOL</t>
+  </si>
+  <si>
+    <t>different invoices to different emails</t>
+  </si>
+  <si>
+    <t>fminv@humber.ca,Margaret.Booth@humber.ca,chantal.joy@humber.ca</t>
+  </si>
+  <si>
+    <t>accounting@insideoutpatio.ca</t>
+  </si>
+  <si>
+    <t>INSIDEPAT</t>
+  </si>
+  <si>
+    <t>ali@jmcbride.net</t>
+  </si>
+  <si>
+    <t>JMCBRIDE</t>
+  </si>
+  <si>
+    <t>admin@lionsgatepropertymgt.ca</t>
+  </si>
+  <si>
+    <t>LIONSGAT</t>
+  </si>
+  <si>
+    <t>NLUISOL</t>
+  </si>
+  <si>
+    <t>marina@northway.cc</t>
+  </si>
+  <si>
+    <t>NORTHW</t>
+  </si>
+  <si>
+    <t>hhashemi@neuerapharma.com</t>
+  </si>
+  <si>
+    <t>NUERALAB</t>
+  </si>
+  <si>
+    <t>accounting@nlisolutions.com</t>
+  </si>
+  <si>
+    <t>documents@onside.ca</t>
+  </si>
+  <si>
+    <t>ONSIDEGTA</t>
+  </si>
+  <si>
+    <t>accounting@mettalifestyles.com</t>
+  </si>
+  <si>
+    <t>QDREAL</t>
+  </si>
+  <si>
+    <t>accountspayable@qaelevator.ca</t>
+  </si>
+  <si>
+    <t>QUALLI</t>
+  </si>
+  <si>
+    <t>irina.loshankova@polarracking.com</t>
+  </si>
+  <si>
+    <t>POLARRACK</t>
+  </si>
+  <si>
+    <t>vivian@rivieraltd.ca</t>
+  </si>
+  <si>
+    <t>RIVIERARES</t>
+  </si>
+  <si>
+    <t>SDM055</t>
+  </si>
+  <si>
+    <t>ssdm1055@shoppersdrugmart.ca,asdm1055@shoppersdrugmart.ca</t>
+  </si>
+  <si>
+    <t>ssdm1279@shoppersdrugmart.ca,asdm1279@shoppersdrugmart.ca</t>
+  </si>
+  <si>
+    <t>SDM279</t>
+  </si>
+  <si>
+    <t>SDM499</t>
+  </si>
+  <si>
+    <t>ssdm499@shoppersdrugmart.ca,asdm499@shoppersdrugmart.ca</t>
+  </si>
+  <si>
+    <t>SDM695</t>
+  </si>
+  <si>
+    <t>ssdm695@shoppersdrugmart.ca,asdm695@shoppersdrugmart.ca</t>
+  </si>
+  <si>
+    <t>SDM698</t>
+  </si>
+  <si>
+    <t>ssdm698@shoppersdrugmart.ca,asdm698@shoppersdrugmart.ca</t>
+  </si>
+  <si>
+    <t>SDM854</t>
+  </si>
+  <si>
+    <t>ssdm854@shoppersdrugmart.ca,asdm854@shoppersdrugmart.ca</t>
+  </si>
+  <si>
+    <t>SDM863</t>
+  </si>
+  <si>
+    <t>ssdm863@shoppersdrugmart.ca,asdm863@shoppersdrugmart.ca</t>
+  </si>
+  <si>
+    <t>SDM925</t>
+  </si>
+  <si>
+    <t>ssdm925@shoppersdrugmart.ca,asdm925@shoppersdrugmart.ca</t>
+  </si>
+  <si>
+    <t>SDM941</t>
+  </si>
+  <si>
+    <t>ssdm941@shoppersdrugmart.ca,asdm941@shoppersdrugmart.ca</t>
+  </si>
+  <si>
+    <t>SDMGLE</t>
+  </si>
+  <si>
+    <t>ssdm907@shoppersdrugmart.ca,asdm907@shoppersdrugmart.ca</t>
+  </si>
+  <si>
+    <t>SDMGOO</t>
+  </si>
+  <si>
+    <t>ssdm905@shoppersdrugmart.ca,asdm905@shoppersdrugmart.ca</t>
+  </si>
+  <si>
+    <t>mon0499@wellwise.ca,afallows@wellwise.ca</t>
+  </si>
+  <si>
+    <t>SDMLAW</t>
+  </si>
+  <si>
+    <t>SHOSCA</t>
+  </si>
+  <si>
+    <t>ssdm811@shoppersdrugmart.ca,asdm811@shoppersdrugmart.ca</t>
+  </si>
+  <si>
+    <t>accounting@sircomachinery.com</t>
+  </si>
+  <si>
+    <t>SIRCOMACH</t>
+  </si>
+  <si>
+    <t>SOLID78</t>
+  </si>
+  <si>
+    <t>orlando@solid78.com</t>
+  </si>
+  <si>
+    <t>THETHE</t>
+  </si>
+  <si>
+    <t>navid@theatrecentre.org</t>
+  </si>
+  <si>
+    <t>TOMMYHILF</t>
+  </si>
+  <si>
+    <t>NARetailOperations@pvh.com</t>
+  </si>
+  <si>
+    <t>TORHYD</t>
+  </si>
+  <si>
+    <t>finance@torglaze.com</t>
+  </si>
+  <si>
+    <t>TORGLAZ</t>
+  </si>
+  <si>
+    <t>ap@torontohydro.com</t>
+  </si>
+  <si>
+    <t>TRIDELEV</t>
+  </si>
+  <si>
+    <t>sfrancis@tridentelevator.com</t>
+  </si>
+  <si>
+    <t>UPTAUD</t>
+  </si>
+  <si>
+    <t>mracktoo@dfcauto.com</t>
+  </si>
+  <si>
+    <t>VALDAV</t>
+  </si>
+  <si>
+    <t>invoices@savers.com</t>
+  </si>
+  <si>
+    <t>WEINJ</t>
+  </si>
+  <si>
+    <t>general@vallionconstruction.com</t>
+  </si>
+  <si>
+    <t>WESGLAS</t>
+  </si>
+  <si>
+    <t>reception@westmetroglass.com</t>
+  </si>
+  <si>
+    <t>Peter.Braybrooke@AvantToronto.com, rob@portamini.com</t>
   </si>
 </sst>
 </file>
@@ -419,18 +713,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D142533-8FFF-4893-98CD-ABAA0ECCF68B}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" customWidth="1"/>
+    <col min="4" max="4" width="44.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,44 +735,466 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{06C2E2B2-8455-4A20-8841-42E995A34179}"/>
-    <hyperlink ref="A3:A5" r:id="rId2" display="kobiatlaslee@gmail.com" xr:uid="{6A1FD8B3-DC0C-47C5-8AFA-253B30D0C344}"/>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{B0A7E8CF-A5F3-4C47-B4C1-114A8FDD09D2}"/>
+    <hyperlink ref="A10" r:id="rId2" xr:uid="{9F558C12-AAFF-4946-9A98-E78A6BF74C67}"/>
+    <hyperlink ref="A11" r:id="rId3" xr:uid="{929B93A3-D904-44B0-B97A-0B42AE4087E4}"/>
+    <hyperlink ref="A13" r:id="rId4" display="contekbuildinggroup@bellnet.ca,gheath.contek@gmail.com" xr:uid="{3721EB2C-1C87-4C28-A17A-880BBE028353}"/>
+    <hyperlink ref="A14" r:id="rId5" xr:uid="{C4EF8D13-B5D4-44AF-9131-D5824EF29281}"/>
+    <hyperlink ref="A15" r:id="rId6" xr:uid="{DFACDC82-8AFA-4E68-941D-D7F3110B934A}"/>
+    <hyperlink ref="A18" r:id="rId7" xr:uid="{F691163B-57B1-47D5-8C06-3D2A916B06B9}"/>
+    <hyperlink ref="D18" r:id="rId8" xr:uid="{D4680330-6A00-49ED-B86C-B1856B91EA1F}"/>
+    <hyperlink ref="A19" r:id="rId9" xr:uid="{F2EF6CE8-5D23-4C66-A746-67B6B7BAC0A5}"/>
+    <hyperlink ref="A22" r:id="rId10" xr:uid="{C1251471-E7C9-49AC-9D17-0788EBF0D0E6}"/>
+    <hyperlink ref="A26" r:id="rId11" xr:uid="{0397A38A-C181-4416-85CA-3828C473B95D}"/>
+    <hyperlink ref="A30" r:id="rId12" xr:uid="{091C0CB8-FBBD-47A0-8634-5D886D710CB0}"/>
+    <hyperlink ref="A31" r:id="rId13" xr:uid="{393EA797-C4D1-4ABF-8467-CA9339F985CA}"/>
+    <hyperlink ref="A32" r:id="rId14" xr:uid="{6BBDF367-19B3-40AD-91EA-29AEB9654D7F}"/>
+    <hyperlink ref="A33" r:id="rId15" xr:uid="{13BC6042-00CE-4465-908B-67F2C37D865E}"/>
+    <hyperlink ref="A34" r:id="rId16" xr:uid="{5A3FDC29-092E-4AEF-9B30-A43D02C2C33D}"/>
+    <hyperlink ref="A35" r:id="rId17" xr:uid="{9E2F1482-B4D7-4C19-A06B-1FE27522EC53}"/>
+    <hyperlink ref="A36" r:id="rId18" xr:uid="{27A71B01-B6E3-4EFA-BCA4-ED2DF3ECF3C7}"/>
+    <hyperlink ref="A37" r:id="rId19" xr:uid="{ECAEDA45-58D9-43E9-810D-F354AD536EF6}"/>
+    <hyperlink ref="A38" r:id="rId20" xr:uid="{279294A5-E353-496A-BEFB-AF504449853B}"/>
+    <hyperlink ref="A39" r:id="rId21" xr:uid="{3C7F5F4B-747A-49C9-A9CC-3B08F88A5FCE}"/>
+    <hyperlink ref="A40" r:id="rId22" xr:uid="{1580B6A4-19D9-4ECC-8324-8CF208E57B5E}"/>
+    <hyperlink ref="A41" r:id="rId23" xr:uid="{B162D68E-BA18-4445-A6D5-5FD47984F6C1}"/>
+    <hyperlink ref="A42" r:id="rId24" xr:uid="{D085DAEE-9A37-48E3-8290-0787988B376C}"/>
+    <hyperlink ref="A43" r:id="rId25" xr:uid="{F8C4D48B-01CB-4BB2-9794-3911854129D3}"/>
+    <hyperlink ref="A45" r:id="rId26" xr:uid="{6D11B3FA-A1C9-4F66-AA13-C058CF4D2B51}"/>
+    <hyperlink ref="A47" r:id="rId27" xr:uid="{1BC8D6D9-75D2-4AF8-A9F5-95FD3E0FFB8B}"/>
+    <hyperlink ref="A51" r:id="rId28" xr:uid="{01290533-95C4-4C84-8E7C-42BDF3669A8C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>